<commit_message>
[FIX]【upgrade to 0.1.4】 fix uncorrent ant2c7n, fix latest menu and init excel
</commit_message>
<xml_diff>
--- a/src/main/resources/script/front/micro-service-init-data.xlsx
+++ b/src/main/resources/script/front/micro-service-init-data.xlsx
@@ -479,7 +479,7 @@
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t>/iam/site-statistics</t>
+          <t>/manager/site-statistics</t>
         </is>
       </c>
       <c r="H8" s="4" t="inlineStr">
@@ -520,7 +520,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>/iam/microservice</t>
+          <t>/manager/microservice</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>/iam/instance</t>
+          <t>/manager/instance</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>/iam/configuration</t>
+          <t>/manager/configuration</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -643,7 +643,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>/iam/route</t>
+          <t>/manager/route</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -684,7 +684,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>/iam/api-test</t>
+          <t>/manager/api-test</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -725,7 +725,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>/iam/api-test</t>
+          <t>/manager/api-test</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -766,7 +766,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>/iam/api-overview</t>
+          <t>/manager/api-overview</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -807,7 +807,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>/iam/api-overview</t>
+          <t>/manager/api-overview</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -848,7 +848,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>/iam/site-statistics</t>
+          <t>/manager/site-statistics</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">

</xml_diff>

<commit_message>
[FIX] init menu, publish 0.17.0
</commit_message>
<xml_diff>
--- a/src/main/resources/script/front/micro-service-init-data.xlsx
+++ b/src/main/resources/script/front/micro-service-init-data.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="D7:N17"/>
+  <dimension ref="D7:N13"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="H10" activeCellId="0" pane="topLeft" sqref="H10"/>
@@ -474,12 +474,12 @@
     <row customHeight="1" ht="12.8" r="8" s="3">
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t>choerodon.route.iam.site-statistics</t>
+          <t>choerodon.route.microservice.micro</t>
         </is>
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t>/manager/site-statistics</t>
+          <t>/manager/microservice</t>
         </is>
       </c>
       <c r="H8" s="4" t="inlineStr">
@@ -494,7 +494,7 @@
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
-          <t>平台统计路由</t>
+          <t>微服务管理路由</t>
         </is>
       </c>
       <c r="K8" s="2" t="inlineStr">
@@ -515,12 +515,12 @@
     <row r="9">
       <c r="F9" t="inlineStr">
         <is>
-          <t>choerodon.route.microservice.micro</t>
+          <t>choerodon.route.microservice.instance-management</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>/manager/microservice</t>
+          <t>/manager/instance</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -535,7 +535,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>微服务管理路由</t>
+          <t>实例管理路由</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -556,12 +556,12 @@
     <row r="10">
       <c r="F10" t="inlineStr">
         <is>
-          <t>choerodon.route.microservice.instance-management</t>
+          <t>choerodon.route.microservice.route-management</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>/manager/instance</t>
+          <t>/manager/route</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -576,7 +576,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>实例管理路由</t>
+          <t>路由管理路由</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -597,12 +597,12 @@
     <row r="11">
       <c r="F11" t="inlineStr">
         <is>
-          <t>choerodon.route.microservice.config-management</t>
+          <t>choerodon.route.microservice.api-management</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>/manager/configuration</t>
+          <t>/manager/api-test</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -617,7 +617,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>配置管理路由</t>
+          <t>平台接口路由</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -638,12 +638,12 @@
     <row r="12">
       <c r="F12" t="inlineStr">
         <is>
-          <t>choerodon.route.microservice.route-management</t>
+          <t>choerodon.route.statistics.api-report</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>/manager/route</t>
+          <t>/manager/api-overview</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -658,7 +658,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>路由管理路由</t>
+          <t>API统计路由</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -679,12 +679,12 @@
     <row r="13">
       <c r="F13" t="inlineStr">
         <is>
-          <t>choerodon.route.microservice.api-management</t>
+          <t>choerodon.route.statistics.menu-report</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>/manager/api-test</t>
+          <t>/manager/site-statistics</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -699,7 +699,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>平台接口路由</t>
+          <t>菜单分析路由</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -714,170 +714,6 @@
         <v>1</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>choerodon.route.api.api-test</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>/manager/api-test</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>manager-service</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>site</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>API测试路由</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>page</t>
-        </is>
-      </c>
-      <c r="L14" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" t="n">
-        <v>1</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>choerodon.route.api.api-overview</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>/manager/api-overview</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>manager-service</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>site</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>API概览路由</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>page</t>
-        </is>
-      </c>
-      <c r="L15" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" t="n">
-        <v>1</v>
-      </c>
-      <c r="N15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>choerodon.route.statistics.api-report</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>/manager/api-overview</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>manager-service</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>site</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>API统计路由</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>page</t>
-        </is>
-      </c>
-      <c r="L16" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" t="n">
-        <v>1</v>
-      </c>
-      <c r="N16" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>choerodon.route.statistics.menu-report</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>/manager/site-statistics</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>manager-service</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>site</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>菜单分析路由</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>page</t>
-        </is>
-      </c>
-      <c r="L17" t="n">
-        <v>0</v>
-      </c>
-      <c r="M17" t="n">
-        <v>1</v>
-      </c>
-      <c r="N17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -902,7 +738,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="D7:O21"/>
+  <dimension ref="D7:O15"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="O8" activeCellId="0" pane="topLeft" sqref="O8"/>
@@ -988,17 +824,17 @@
     <row customHeight="1" ht="12.8" r="8" s="3">
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t>choerodon.code.iam</t>
+          <t>choerodon.code.microservice</t>
         </is>
       </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
-          <t>平台设置</t>
+          <t>平台服务</t>
         </is>
       </c>
       <c r="H8" s="4" t="inlineStr">
         <is>
-          <t>platform settings</t>
+          <t>Site Service</t>
         </is>
       </c>
       <c r="I8" s="2" t="n"/>
@@ -1024,32 +860,32 @@
       </c>
       <c r="N8" s="2" t="inlineStr">
         <is>
-          <t>IAM</t>
+          <t>pages</t>
         </is>
       </c>
       <c r="O8" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
       <c r="F9" t="inlineStr">
         <is>
-          <t>choerodon.code.iam.site-statistics</t>
+          <t>choerodon.code.microservice.micro</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>平台统计</t>
+          <t>微服务管理</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Site Statistics</t>
+          <t>Microservice Management</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>choerodon.route.iam.site-statistics</t>
+          <t>choerodon.route.microservice.micro</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1059,7 +895,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>choerodon.code.iam</t>
+          <t>choerodon.code.microservice</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1074,39 +910,44 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>timeline</t>
+          <t>microservice</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="F10" t="inlineStr">
         <is>
+          <t>choerodon.code.microservice.instance-management</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>实例管理</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Instance Management</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>choerodon.route.microservice.instance-management</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>manager-service</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
           <t>choerodon.code.microservice</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>平台服务</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Site Service</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>manager-service</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>choerodon.code.top.site</t>
-        </is>
-      </c>
       <c r="L10" t="inlineStr">
         <is>
           <t>site</t>
@@ -1114,37 +955,37 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>menu</t>
+          <t>menu_item</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>pages</t>
+          <t>instance_outline</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="F11" t="inlineStr">
         <is>
-          <t>choerodon.code.microservice.micro</t>
+          <t>choerodon.code.microservice.route-management</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>微服务管理</t>
+          <t>路由管理</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Microservice Management</t>
+          <t>Route Management</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>choerodon.route.microservice.micro</t>
+          <t>choerodon.route.microservice.route-management</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1169,32 +1010,32 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>microservice</t>
+          <t>routeroutline</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
       <c r="F12" t="inlineStr">
         <is>
-          <t>choerodon.code.microservice.instance-management</t>
+          <t>choerodon.code.microservice.api-management</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>实例管理</t>
+          <t>平台接口</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Instance Management</t>
+          <t>Api Management</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>choerodon.route.microservice.instance-management</t>
+          <t>choerodon.route.microservice.api-management</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1219,32 +1060,27 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>instance_outline</t>
+          <t>API</t>
         </is>
       </c>
       <c r="O12" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
       <c r="F13" t="inlineStr">
         <is>
-          <t>choerodon.code.microservice.config-management</t>
+          <t>choerodon.code.statistics</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>配置管理</t>
+          <t>平台统计</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Config Management</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>choerodon.route.microservice.config-management</t>
+          <t>Site Statistics</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1254,7 +1090,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>choerodon.code.microservice</t>
+          <t>choerodon.code.top.site</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1264,37 +1100,37 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>menu_item</t>
+          <t>menu</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>settings_input_composite</t>
+          <t>bar_chart</t>
         </is>
       </c>
       <c r="O13" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
       <c r="F14" t="inlineStr">
         <is>
-          <t>choerodon.code.microservice.route-management</t>
+          <t>choerodon.code.statistics.api-report</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>路由管理</t>
+          <t>API统计</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Route Management</t>
+          <t>Api Overview</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>choerodon.route.microservice.route-management</t>
+          <t>choerodon.route.statistics.api-report</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1304,7 +1140,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>choerodon.code.microservice</t>
+          <t>choerodon.code.statistics</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1319,32 +1155,32 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>routeroutline</t>
+          <t>dashboard</t>
         </is>
       </c>
       <c r="O14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
       <c r="F15" t="inlineStr">
         <is>
-          <t>choerodon.code.microservice.api-management</t>
+          <t>choerodon.code.statistics.menu-report</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>平台接口</t>
+          <t>菜单分析</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Api Management</t>
+          <t>Menu Report</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>choerodon.route.microservice.api-management</t>
+          <t>choerodon.route.statistics.menu-report</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1354,7 +1190,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>choerodon.code.microservice</t>
+          <t>choerodon.code.statistics</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1369,300 +1205,10 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>API</t>
+          <t>timeline</t>
         </is>
       </c>
       <c r="O15" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>choerodon.code.api</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>API管理</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>API Manage</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>manager-service</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>choerodon.code.top.site</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>site</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>menu</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>API</t>
-        </is>
-      </c>
-      <c r="O16" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>choerodon.code.api.api-test</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>API测试</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>API Test</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>choerodon.route.api.api-test</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>manager-service</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>choerodon.code.api</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>site</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>menu_item</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>APItest</t>
-        </is>
-      </c>
-      <c r="O17" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>choerodon.code.api.api-overview</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>API概览</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>API Overview</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>choerodon.route.api.api-overview</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>manager-service</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>choerodon.code.api</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>site</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>menu_item</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>dashboard</t>
-        </is>
-      </c>
-      <c r="O18" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>choerodon.code.statistics</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>平台统计</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Site Statistics</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>manager-service</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>choerodon.code.top.site</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>site</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>menu</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>bar_chart</t>
-        </is>
-      </c>
-      <c r="O19" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>choerodon.code.statistics.api-report</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>API统计</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Api Overview</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>choerodon.route.statistics.api-report</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>manager-service</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>choerodon.code.statistics</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>site</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>menu_item</t>
-        </is>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>dashboard</t>
-        </is>
-      </c>
-      <c r="O20" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>choerodon.code.statistics.menu-report</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>菜单分析</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Menu Report</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>choerodon.route.statistics.menu-report</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>manager-service</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>choerodon.code.statistics</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>site</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>menu_item</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>timeline</t>
-        </is>
-      </c>
-      <c r="O21" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1687,7 +1233,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="D7:G32"/>
+  <dimension ref="D7:G20"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="E25" activeCellId="0" pane="topLeft" sqref="E25"/>
@@ -1728,24 +1274,24 @@
     <row customHeight="1" ht="12.8" r="8" s="3">
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>choerodon.code.iam.site-statistics</t>
+          <t>choerodon.code.microservice.micro</t>
         </is>
       </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
-          <t>manager-service.statistic.queryMenuClick</t>
+          <t>manager-service.service.pageManager</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="F9" t="inlineStr">
         <is>
-          <t>choerodon.code.microservice.micro</t>
+          <t>choerodon.code.microservice.instance-management</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>manager-service.service.pageManager</t>
+          <t>manager-service.instance.list</t>
         </is>
       </c>
     </row>
@@ -1757,269 +1303,125 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>manager-service.instance.list</t>
+          <t>manager-service.instance.query</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="F11" t="inlineStr">
         <is>
-          <t>choerodon.code.microservice.instance-management</t>
+          <t>choerodon.code.microservice.route-management</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>manager-service.instance.query</t>
+          <t>manager-service.route.list</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="F12" t="inlineStr">
         <is>
-          <t>choerodon.code.microservice.config-management</t>
+          <t>choerodon.code.microservice.route-management</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>manager-service.config.query</t>
+          <t>manager-service.route.create</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="F13" t="inlineStr">
         <is>
-          <t>choerodon.code.microservice.config-management</t>
+          <t>choerodon.code.microservice.route-management</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>manager-service.config.create</t>
+          <t>manager-service.route.update</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="F14" t="inlineStr">
         <is>
-          <t>choerodon.code.microservice.config-management</t>
+          <t>choerodon.code.microservice.route-management</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>manager-service.config.delete</t>
+          <t>manager-service.route.delete</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="F15" t="inlineStr">
         <is>
-          <t>choerodon.code.microservice.config-management</t>
+          <t>choerodon.code.microservice.api-management</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>manager-service.config.queryYaml</t>
+          <t>manager-service.api.queryTreeMenu</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="F16" t="inlineStr">
         <is>
-          <t>choerodon.code.microservice.config-management</t>
+          <t>choerodon.code.microservice.api-management</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>manager-service.config.updateConfig</t>
+          <t>manager-service.api.queryPathDetail</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="F17" t="inlineStr">
         <is>
-          <t>choerodon.code.microservice.config-management</t>
+          <t>choerodon.code.statistics.api-report</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>manager-service.config.updateConfigDefault</t>
+          <t>manager-service.api.queryInstancesAndApiCount</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="F18" t="inlineStr">
         <is>
-          <t>choerodon.code.microservice.route-management</t>
+          <t>choerodon.code.statistics.api-report</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>manager-service.route.list</t>
+          <t>manager-service.api.queryApiInvoke</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="F19" t="inlineStr">
         <is>
-          <t>choerodon.code.microservice.route-management</t>
+          <t>choerodon.code.statistics.api-report</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>manager-service.route.create</t>
+          <t>manager-service.api.queryServiceInvoke</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="F20" t="inlineStr">
         <is>
-          <t>choerodon.code.microservice.route-management</t>
+          <t>choerodon.code.statistics.menu-report</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
-        <is>
-          <t>manager-service.route.update</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>choerodon.code.microservice.route-management</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>manager-service.route.delete</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>choerodon.code.microservice.api-management</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>manager-service.api.queryTreeMenu</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>choerodon.code.microservice.api-management</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>manager-service.api.queryPathDetail</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>choerodon.code.api.api-test</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>manager-service.api.queryTreeMenu</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>choerodon.code.api.api-test</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>manager-service.api.queryPathDetail</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>choerodon.code.api.api-overview</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>manager-service.api.queryInstancesAndApiCount</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>choerodon.code.api.api-overview</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>manager-service.api.queryApiInvoke</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>choerodon.code.api.api-overview</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>manager-service.api.queryServiceInvoke</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>choerodon.code.statistics.api-report</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>manager-service.api.queryInstancesAndApiCount</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>choerodon.code.statistics.api-report</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>manager-service.api.queryApiInvoke</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>choerodon.code.statistics.api-report</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>manager-service.api.queryServiceInvoke</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>choerodon.code.statistics.menu-report</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
         <is>
           <t>manager-service.statistic.queryMenuClick</t>
         </is>

</xml_diff>